<commit_message>
Update Optimiser Summary Statistics with rand.xlsx
</commit_message>
<xml_diff>
--- a/examples/DOE/Optimiser Summary Statistics with rand.xlsx
+++ b/examples/DOE/Optimiser Summary Statistics with rand.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubai\Documents\Programming\AI3SD\edbo\examples\DOE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FFB1A75-A5A1-4484-9EB2-935ECDC89C92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686A9239-116D-4D08-B15D-F3117A4A01B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimiser Summary Statistics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -67,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,6 +605,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3A0CA3"/>
+      <color rgb="FFF72585"/>
+      <color rgb="FF7209B7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -622,29 +640,220 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Random</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F72585"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Optimiser Summary Statistics'!$I$32:$I$41</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>0.29839906166072305</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.32102647865869255</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.29698484809834996</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.33092597359530423</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.3139554108468271</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.32668333290818496</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.24890158697766471</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.35921024484276615</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.32951176003293114</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.27435743110038041</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Optimiser Summary Statistics'!$I$32:$I$41</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>0.29839906166072305</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.32102647865869255</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.29698484809834996</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.33092597359530423</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.3139554108468271</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.32668333290818496</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.24890158697766471</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.35921024484276615</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.32951176003293114</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.27435743110038041</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Optimiser Summary Statistics'!$C$32:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Optimiser Summary Statistics'!$E$32:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>95.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>95.73</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95.82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A396-406A-A17D-584945F0D685}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Expected improvement</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:srgbClr val="7209B7"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
-            <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
@@ -730,14 +939,14 @@
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>'Optimiser Summary Statistics'!$C$2:$C$11</c:f>
               <c:numCache>
@@ -775,8 +984,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>'Optimiser Summary Statistics'!$E$2:$E$11</c:f>
               <c:numCache>
@@ -814,211 +1023,10 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A396-406A-A17D-584945F0D685}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Random</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Optimiser Summary Statistics'!$I$32:$I$41</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
-                  <c:pt idx="0">
-                    <c:v>0.29839906166072305</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.32102647865869255</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.29698484809834996</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.33092597359530423</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.3139554108468271</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0.32668333290818496</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0.24890158697766471</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.35921024484276615</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0.32951176003293114</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0.27435743110038041</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'Optimiser Summary Statistics'!$I$32:$I$41</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
-                  <c:pt idx="0">
-                    <c:v>0.29839906166072305</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.32102647865869255</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.29698484809834996</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.33092597359530423</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.3139554108468271</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0.32668333290818496</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0.24890158697766471</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.35921024484276615</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0.32951176003293114</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0.27435743110038041</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Optimiser Summary Statistics'!$C$32:$C$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Optimiser Summary Statistics'!$E$32:$E$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>95.71</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>95.37</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>95.54</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>95.52</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>95.63</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>95.55</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>95.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>96.15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>95.73</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>95.82</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A396-406A-A17D-584945F0D685}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1029,19 +1037,16 @@
             <c:v>Thompson sampling</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:srgbClr val="3A0CA3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
-            <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
@@ -1127,17 +1132,14 @@
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>'Optimiser Summary Statistics'!$C$12:$C$21</c:f>
               <c:numCache>
@@ -1175,8 +1177,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>'Optimiser Summary Statistics'!$E$12:$E$21</c:f>
               <c:numCache>
@@ -1214,8 +1216,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-A396-406A-A17D-584945F0D685}"/>
@@ -1230,15 +1231,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="453355520"/>
         <c:axId val="453356176"/>
-      </c:scatterChart>
-      <c:valAx>
+      </c:barChart>
+      <c:catAx>
         <c:axId val="453355520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10"/>
-          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1295,8 +1295,11 @@
         </c:txPr>
         <c:crossAx val="453356176"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="453356176"/>
         <c:scaling>
@@ -1320,6 +1323,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Max</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> observed yield, averaged</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1359,7 +1421,7 @@
         </c:txPr>
         <c:crossAx val="453355520"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2337,11 +2399,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Changed colour of thompson sampling to lighter blue to make black more visible
</commit_message>
<xml_diff>
--- a/examples/DOE/Optimiser Summary Statistics with rand.xlsx
+++ b/examples/DOE/Optimiser Summary Statistics with rand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubai\Documents\Programming\AI3SD\edbo\examples\DOE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686A9239-116D-4D08-B15D-F3117A4A01B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AD0615-19FC-444A-B1A3-A69911504798}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -607,6 +607,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4361EE"/>
+      <color rgb="FF4CC9F0"/>
       <color rgb="FF3A0CA3"/>
       <color rgb="FFF72585"/>
       <color rgb="FF7209B7"/>
@@ -1038,7 +1040,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="3A0CA3"/>
+              <a:srgbClr val="4361EE"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1323,65 +1325,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Max</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> observed yield, averaged</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1433,6 +1376,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13525788199827529"/>
+          <c:y val="0.85378580217725486"/>
+          <c:w val="0.72948401773961169"/>
+          <c:h val="8.2589861186418534E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2403,7 +2356,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>